<commit_message>
updated BoM and get started
</commit_message>
<xml_diff>
--- a/docs/hardware/Helmoro_BoM_14-07-2023.xlsx
+++ b/docs/hardware/Helmoro_BoM_14-07-2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHE\Documents\Git_Data\HelMoRo\docs\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC8EE4C-DE37-47F9-8778-EEC6886CF0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897425D0-1D61-4501-9CEF-62B006C76B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D43A7108-50A9-4FCF-900B-676A8BDC7C7C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="180">
   <si>
     <t>POS</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t xml:space="preserve">Battery Protection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
   </si>
 </sst>
 </file>
@@ -690,12 +693,26 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="653">
-    <dxf>
+  <dxfs count="655">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -717,6 +734,31 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5638,20 +5680,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC433D18-8D56-470A-8DB2-FE2100CD4686}" name="Table1" displayName="Table1" ref="A1:H54" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18">
-  <autoFilter ref="A1:H54" xr:uid="{AB8CB7B2-62CE-4583-9267-907B832DB447}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC433D18-8D56-470A-8DB2-FE2100CD4686}" name="Table1" displayName="Table1" ref="A1:I54" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20">
+  <autoFilter ref="A1:I54" xr:uid="{AB8CB7B2-62CE-4583-9267-907B832DB447}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H54">
     <sortCondition ref="A1:A54"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8C720362-16ED-4641-BAC4-38765F6008BF}" name="POS" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{E4EF20A8-BAA7-4285-8E2C-1FF15F4D9DE0}" name="QTY" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{7C114C88-4C53-4A01-875E-42C9A5D3836B}" name="DOCUMENT-NR." dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{F56A10FA-89C2-4781-AECC-93B30002C92E}" name="DESCRIPTION" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{DC161508-7262-4AC6-90ED-F4CD4C38651A}" name="Manufacturing type" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{15467916-B419-479D-A3A9-C6B2B5C762DF}" name="PRODUCT CODE" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{2349CBB5-C81B-4DFD-9B9F-CC6E1EB0C9BF}" name="SUPPLIER" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{36592479-8EA8-4D42-8DFF-452C7024B605}" name="Price per unit (CHF)" dataDxfId="3" totalsRowDxfId="2"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{8C720362-16ED-4641-BAC4-38765F6008BF}" name="POS" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{E4EF20A8-BAA7-4285-8E2C-1FF15F4D9DE0}" name="QTY" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{7C114C88-4C53-4A01-875E-42C9A5D3836B}" name="DOCUMENT-NR." dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{F56A10FA-89C2-4781-AECC-93B30002C92E}" name="DESCRIPTION" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{DC161508-7262-4AC6-90ED-F4CD4C38651A}" name="Manufacturing type" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{15467916-B419-479D-A3A9-C6B2B5C762DF}" name="PRODUCT CODE" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{2349CBB5-C81B-4DFD-9B9F-CC6E1EB0C9BF}" name="SUPPLIER" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{36592479-8EA8-4D42-8DFF-452C7024B605}" name="Price per unit (CHF)" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{C3872188-6A6F-4DEA-BDF2-4169887BB0CD}" name="Total" dataDxfId="0" totalsRowDxfId="1">
+      <calculatedColumnFormula>B2*H2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5666,9 +5711,9 @@
     <tableColumn id="3" xr3:uid="{A8C4F21C-CD18-4C55-8F37-A63DC3DADA2A}" name="Length [m]"/>
     <tableColumn id="4" xr3:uid="{58450646-C7B3-41F9-9EA9-C5AC13C9F0E1}" name="QTY to ZHR"/>
     <tableColumn id="5" xr3:uid="{7591EFD4-7391-4754-8536-9BFADAB2E4F8}" name="QTY to BOS"/>
-    <tableColumn id="6" xr3:uid="{62F124C5-9852-4F6A-9A5B-7833BB832B2B}" name="TOTAL QTY" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{62F124C5-9852-4F6A-9A5B-7833BB832B2B}" name="TOTAL QTY" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{96FA4321-6955-4909-B76A-703878A5516D}" name="Cost/part [CHF]"/>
-    <tableColumn id="8" xr3:uid="{F9E937AD-E464-40D7-87A7-E2D2618ABCD4}" name="Total [CHF]" totalsRowFunction="sum" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{F9E937AD-E464-40D7-87A7-E2D2618ABCD4}" name="Total [CHF]" totalsRowFunction="sum" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5971,10 +6016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C6E063-1877-40DA-BDBC-FD081DB60E9D}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5989,7 +6034,7 @@
     <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6014,8 +6059,11 @@
       <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -6040,8 +6088,12 @@
       <c r="H2" s="7">
         <v>100</v>
       </c>
+      <c r="I2" s="7">
+        <f t="shared" ref="I2:I33" si="0">B2*H2</f>
+        <v>100</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -6066,8 +6118,12 @@
       <c r="H3" s="7">
         <v>80</v>
       </c>
+      <c r="I3" s="7">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -6089,11 +6145,14 @@
       <c r="G4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>163</v>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -6115,11 +6174,14 @@
       <c r="G5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>163</v>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -6144,8 +6206,12 @@
       <c r="H6" s="7">
         <v>30</v>
       </c>
+      <c r="I6" s="7">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -6170,8 +6236,12 @@
       <c r="H7" s="7">
         <v>3</v>
       </c>
+      <c r="I7" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -6196,8 +6266,12 @@
       <c r="H8" s="7">
         <v>4</v>
       </c>
+      <c r="I8" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -6219,11 +6293,15 @@
       <c r="G9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>163</v>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -6248,8 +6326,12 @@
       <c r="H10" s="7">
         <v>71.3</v>
       </c>
+      <c r="I10" s="7">
+        <f t="shared" si="0"/>
+        <v>71.3</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -6271,11 +6353,15 @@
       <c r="G11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>163</v>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -6297,11 +6383,15 @@
       <c r="G12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>163</v>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -6324,8 +6414,12 @@
       <c r="H13" s="7">
         <v>70</v>
       </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>14</v>
       </c>
@@ -6350,8 +6444,12 @@
       <c r="H14" s="7">
         <v>39</v>
       </c>
+      <c r="I14" s="7">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
     </row>
-    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>15</v>
       </c>
@@ -6376,8 +6474,12 @@
       <c r="H15" s="7">
         <v>113</v>
       </c>
+      <c r="I15" s="7">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>16</v>
       </c>
@@ -6402,8 +6504,12 @@
       <c r="H16" s="7">
         <v>15</v>
       </c>
+      <c r="I16" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>17</v>
       </c>
@@ -6425,9 +6531,15 @@
       <c r="G17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>18</v>
       </c>
@@ -6449,9 +6561,15 @@
       <c r="G18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>19</v>
       </c>
@@ -6476,8 +6594,12 @@
       <c r="H19" s="7">
         <v>320</v>
       </c>
+      <c r="I19" s="7">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>20</v>
       </c>
@@ -6499,11 +6621,15 @@
       <c r="G20" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>163</v>
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>21</v>
       </c>
@@ -6528,8 +6654,12 @@
       <c r="H21" s="7">
         <v>200</v>
       </c>
+      <c r="I21" s="7">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>22</v>
       </c>
@@ -6551,11 +6681,15 @@
       <c r="G22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>163</v>
+      <c r="H22" s="7">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>23</v>
       </c>
@@ -6577,11 +6711,15 @@
       <c r="G23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>163</v>
+      <c r="H23" s="6">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>24</v>
       </c>
@@ -6606,8 +6744,12 @@
       <c r="H24" s="7">
         <v>3</v>
       </c>
+      <c r="I24" s="7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
     </row>
-    <row r="25" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>25</v>
       </c>
@@ -6632,8 +6774,12 @@
       <c r="H25" s="7">
         <v>38</v>
       </c>
+      <c r="I25" s="7">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>26</v>
       </c>
@@ -6649,9 +6795,15 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="H26" s="7">
+        <v>0</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>27</v>
       </c>
@@ -6669,9 +6821,15 @@
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="H27" s="7">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>28</v>
       </c>
@@ -6689,9 +6847,15 @@
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="H28" s="7">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>29</v>
       </c>
@@ -6709,9 +6873,15 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="H29" s="7">
+        <v>0</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>30</v>
       </c>
@@ -6729,9 +6899,15 @@
       <c r="G30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="7"/>
+      <c r="H30" s="7">
+        <v>0</v>
+      </c>
+      <c r="I30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>31</v>
       </c>
@@ -6751,9 +6927,15 @@
       <c r="G31" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="H31" s="7"/>
+      <c r="H31" s="7">
+        <v>13</v>
+      </c>
+      <c r="I31" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>32</v>
       </c>
@@ -6778,8 +6960,12 @@
       <c r="H32" s="7">
         <v>100</v>
       </c>
+      <c r="I32" s="7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>33</v>
       </c>
@@ -6804,8 +6990,12 @@
       <c r="H33" s="7">
         <v>50</v>
       </c>
+      <c r="I33" s="7">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
     </row>
-    <row r="34" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>34</v>
       </c>
@@ -6830,8 +7020,12 @@
       <c r="H34" s="7">
         <v>50</v>
       </c>
+      <c r="I34" s="7">
+        <f t="shared" ref="I34:I65" si="1">B34*H34</f>
+        <v>50</v>
+      </c>
     </row>
-    <row r="35" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>35</v>
       </c>
@@ -6856,8 +7050,12 @@
       <c r="H35" s="7">
         <v>11.3</v>
       </c>
+      <c r="I35" s="7">
+        <f t="shared" si="1"/>
+        <v>22.6</v>
+      </c>
     </row>
-    <row r="36" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>36</v>
       </c>
@@ -6882,8 +7080,12 @@
       <c r="H36" s="7">
         <v>6</v>
       </c>
+      <c r="I36" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="37" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>37</v>
       </c>
@@ -6905,11 +7107,15 @@
       <c r="G37" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="H37" s="7" t="s">
-        <v>163</v>
+      <c r="H37" s="7">
+        <v>0</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>38</v>
       </c>
@@ -6931,11 +7137,15 @@
       <c r="G38" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="H38" s="7" t="s">
-        <v>163</v>
+      <c r="H38" s="7">
+        <v>5.15</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="1"/>
+        <v>5.15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>39</v>
       </c>
@@ -6957,11 +7167,15 @@
       <c r="G39" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="H39" s="7" t="s">
-        <v>163</v>
+      <c r="H39" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="126" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>40</v>
       </c>
@@ -6983,11 +7197,15 @@
       <c r="G40" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="H40" s="7" t="s">
-        <v>163</v>
+      <c r="H40" s="7">
+        <v>3</v>
+      </c>
+      <c r="I40" s="7">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>41</v>
       </c>
@@ -7009,11 +7227,15 @@
       <c r="G41" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H41" s="7" t="s">
-        <v>163</v>
+      <c r="H41" s="7">
+        <v>0</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>42</v>
       </c>
@@ -7035,11 +7257,15 @@
       <c r="G42" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H42" s="7" t="s">
-        <v>163</v>
+      <c r="H42" s="7">
+        <v>0</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43</v>
       </c>
@@ -7061,11 +7287,15 @@
       <c r="G43" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="7" t="s">
-        <v>163</v>
+      <c r="H43" s="7">
+        <v>0</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>44</v>
       </c>
@@ -7087,11 +7317,15 @@
       <c r="G44" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="7" t="s">
-        <v>163</v>
+      <c r="H44" s="7">
+        <v>0</v>
+      </c>
+      <c r="I44" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>45</v>
       </c>
@@ -7113,11 +7347,15 @@
       <c r="G45" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="7" t="s">
-        <v>163</v>
+      <c r="H45" s="7">
+        <v>0</v>
+      </c>
+      <c r="I45" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>46</v>
       </c>
@@ -7139,11 +7377,15 @@
       <c r="G46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H46" s="7" t="s">
-        <v>163</v>
+      <c r="H46" s="7">
+        <v>0</v>
+      </c>
+      <c r="I46" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>47</v>
       </c>
@@ -7165,11 +7407,15 @@
       <c r="G47" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H47" s="6" t="s">
-        <v>163</v>
+      <c r="H47" s="6">
+        <v>0</v>
+      </c>
+      <c r="I47" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>48</v>
       </c>
@@ -7191,11 +7437,15 @@
       <c r="G48" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>163</v>
+      <c r="H48" s="7">
+        <v>0</v>
+      </c>
+      <c r="I48" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>49</v>
       </c>
@@ -7217,11 +7467,15 @@
       <c r="G49" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H49" s="7" t="s">
-        <v>163</v>
+      <c r="H49" s="7">
+        <v>0</v>
+      </c>
+      <c r="I49" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>50</v>
       </c>
@@ -7243,11 +7497,15 @@
       <c r="G50" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="H50" s="7" t="s">
-        <v>163</v>
+      <c r="H50" s="7">
+        <v>0</v>
+      </c>
+      <c r="I50" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>51</v>
       </c>
@@ -7269,11 +7527,15 @@
       <c r="G51" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="H51" s="7" t="s">
-        <v>163</v>
+      <c r="H51" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="I51" s="7">
+        <f t="shared" si="1"/>
+        <v>3.4</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>52</v>
       </c>
@@ -7295,11 +7557,15 @@
       <c r="G52" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H52" s="7" t="s">
-        <v>163</v>
+      <c r="H52" s="7">
+        <v>0</v>
+      </c>
+      <c r="I52" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>53</v>
       </c>
@@ -7321,11 +7587,15 @@
       <c r="G53" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H53" s="7" t="s">
-        <v>163</v>
+      <c r="H53" s="7">
+        <v>0</v>
+      </c>
+      <c r="I53" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>54</v>
       </c>
@@ -7347,11 +7617,24 @@
       <c r="G54" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H54" s="7" t="s">
-        <v>163</v>
+      <c r="H54" s="7">
+        <v>0</v>
+      </c>
+      <c r="I54" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H56" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I56" s="3">
+        <f>SUM(Table1[Total])</f>
+        <v>1555.8500000000001</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{2DB68C68-C8A3-4D36-85A2-312BD3E62D69}">
@@ -7361,2214 +7644,2214 @@
   </customSheetViews>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="G25:G31">
-    <cfRule type="expression" dxfId="652" priority="833">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="651" priority="834">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="650" priority="835">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="649" priority="836">
+    <cfRule type="expression" dxfId="654" priority="833">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="653" priority="834">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="652" priority="835">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="651" priority="836">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:H13 G5 F6:H8 E12 G11:G12 F14:H16 G22 H32 G33:H33 F37:G40 G41 G43 F44:G44 G45:G46 G48 F23:H31 E42:G42 E47:H47 E43 E41 E33 A2:B54">
-    <cfRule type="expression" dxfId="648" priority="841">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="647" priority="842">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="646" priority="843">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="645" priority="844">
+    <cfRule type="expression" dxfId="650" priority="841">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="649" priority="842">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="648" priority="843">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="647" priority="844">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:G31">
-    <cfRule type="expression" dxfId="644" priority="845">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="643" priority="846">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="642" priority="847">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="641" priority="848">
+    <cfRule type="expression" dxfId="646" priority="845">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="645" priority="846">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="644" priority="847">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="643" priority="848">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18 G52:G54 E2:H4 E10:H10 E17:H17 E19:G19 F20:G20 E21:G21 E9 G9 E35:H36">
-    <cfRule type="expression" dxfId="640" priority="857">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="639" priority="858">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="638" priority="859">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="637" priority="860">
+    <cfRule type="expression" dxfId="642" priority="857">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="641" priority="858">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="640" priority="859">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="639" priority="860">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="expression" dxfId="636" priority="953">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="635" priority="954">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="634" priority="955">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="633" priority="956">
+    <cfRule type="expression" dxfId="638" priority="953">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="637" priority="954">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="636" priority="955">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="635" priority="956">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="expression" dxfId="632" priority="1005">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="631" priority="1006">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="630" priority="1007">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="629" priority="1008">
+    <cfRule type="expression" dxfId="634" priority="1005">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="633" priority="1006">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="632" priority="1007">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="631" priority="1008">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="628" priority="677">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="627" priority="678">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="626" priority="679">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="625" priority="680">
+    <cfRule type="expression" dxfId="630" priority="677">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="629" priority="678">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="628" priority="679">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="627" priority="680">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="624" priority="673">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="623" priority="674">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="622" priority="675">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="621" priority="676">
+    <cfRule type="expression" dxfId="626" priority="673">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="625" priority="674">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="624" priority="675">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="623" priority="676">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="620" priority="669">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="619" priority="670">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="618" priority="671">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="617" priority="672">
+    <cfRule type="expression" dxfId="622" priority="669">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="621" priority="670">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="620" priority="671">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="619" priority="672">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="616" priority="665">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="615" priority="666">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="614" priority="667">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="613" priority="668">
+    <cfRule type="expression" dxfId="618" priority="665">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="617" priority="666">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="616" priority="667">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="615" priority="668">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="612" priority="661">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="611" priority="662">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="610" priority="663">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="609" priority="664">
+    <cfRule type="expression" dxfId="614" priority="661">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="613" priority="662">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="612" priority="663">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="611" priority="664">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="608" priority="657">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="607" priority="658">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="606" priority="659">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="605" priority="660">
+    <cfRule type="expression" dxfId="610" priority="657">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="609" priority="658">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="608" priority="659">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="607" priority="660">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="604" priority="653">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="603" priority="654">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="602" priority="655">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="601" priority="656">
+    <cfRule type="expression" dxfId="606" priority="653">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="605" priority="654">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="604" priority="655">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="603" priority="656">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="600" priority="649">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="599" priority="650">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="598" priority="651">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="597" priority="652">
+    <cfRule type="expression" dxfId="602" priority="649">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="601" priority="650">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="600" priority="651">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="599" priority="652">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="596" priority="645">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="595" priority="646">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="594" priority="647">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="593" priority="648">
+    <cfRule type="expression" dxfId="598" priority="645">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="597" priority="646">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="596" priority="647">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="595" priority="648">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="592" priority="641">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="591" priority="642">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="590" priority="643">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="589" priority="644">
+    <cfRule type="expression" dxfId="594" priority="641">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="593" priority="642">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="592" priority="643">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="591" priority="644">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="588" priority="637">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="587" priority="638">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="586" priority="639">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="585" priority="640">
+    <cfRule type="expression" dxfId="590" priority="637">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="589" priority="638">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="588" priority="639">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="587" priority="640">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="584" priority="625">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="583" priority="626">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="582" priority="627">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="581" priority="628">
+    <cfRule type="expression" dxfId="586" priority="625">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="585" priority="626">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="584" priority="627">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="583" priority="628">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="580" priority="621">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="579" priority="622">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="578" priority="623">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="577" priority="624">
+    <cfRule type="expression" dxfId="582" priority="621">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="581" priority="622">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="580" priority="623">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="579" priority="624">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="576" priority="617">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="575" priority="618">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="574" priority="619">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="573" priority="620">
+    <cfRule type="expression" dxfId="578" priority="617">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="577" priority="618">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="576" priority="619">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="575" priority="620">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="572" priority="613">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="571" priority="614">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="570" priority="615">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="569" priority="616">
+    <cfRule type="expression" dxfId="574" priority="613">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="573" priority="614">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="572" priority="615">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="571" priority="616">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="568" priority="609">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="567" priority="610">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="566" priority="611">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="565" priority="612">
+    <cfRule type="expression" dxfId="570" priority="609">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="569" priority="610">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="568" priority="611">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="567" priority="612">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="564" priority="605">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="563" priority="606">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="562" priority="607">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="561" priority="608">
+    <cfRule type="expression" dxfId="566" priority="605">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="565" priority="606">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="564" priority="607">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="563" priority="608">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" dxfId="560" priority="601">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="559" priority="602">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="558" priority="603">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="557" priority="604">
+    <cfRule type="expression" dxfId="562" priority="601">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="561" priority="602">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="560" priority="603">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="559" priority="604">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="556" priority="597">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="555" priority="598">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="554" priority="599">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="553" priority="600">
+    <cfRule type="expression" dxfId="558" priority="597">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="557" priority="598">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="556" priority="599">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="555" priority="600">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="552" priority="593">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="551" priority="594">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="550" priority="595">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="549" priority="596">
+    <cfRule type="expression" dxfId="554" priority="593">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="553" priority="594">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="552" priority="595">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="551" priority="596">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="548" priority="589">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="547" priority="590">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="546" priority="591">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="545" priority="592">
+    <cfRule type="expression" dxfId="550" priority="589">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="549" priority="590">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="548" priority="591">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="547" priority="592">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="544" priority="585">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="543" priority="586">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="542" priority="587">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="541" priority="588">
+    <cfRule type="expression" dxfId="546" priority="585">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="545" priority="586">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="544" priority="587">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="543" priority="588">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="540" priority="581">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="539" priority="582">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="538" priority="583">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="537" priority="584">
+    <cfRule type="expression" dxfId="542" priority="581">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="541" priority="582">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="540" priority="583">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="539" priority="584">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E26 E30:E31">
-    <cfRule type="expression" dxfId="536" priority="577">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="535" priority="578">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="534" priority="579">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="533" priority="580">
+    <cfRule type="expression" dxfId="538" priority="577">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="537" priority="578">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="536" priority="579">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="535" priority="580">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" dxfId="532" priority="561">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="531" priority="562">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="530" priority="563">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="529" priority="564">
+    <cfRule type="expression" dxfId="534" priority="561">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="533" priority="562">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="532" priority="563">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="531" priority="564">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="expression" dxfId="528" priority="557">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="527" priority="558">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="526" priority="559">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="525" priority="560">
+    <cfRule type="expression" dxfId="530" priority="557">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="529" priority="558">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="528" priority="559">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="527" priority="560">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="expression" dxfId="524" priority="553">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="523" priority="554">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="522" priority="555">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="521" priority="556">
+    <cfRule type="expression" dxfId="526" priority="553">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="525" priority="554">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="524" priority="555">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="523" priority="556">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33">
-    <cfRule type="expression" dxfId="520" priority="549">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="519" priority="550">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="518" priority="551">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="517" priority="552">
+    <cfRule type="expression" dxfId="522" priority="549">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="521" priority="550">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="520" priority="551">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="519" priority="552">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="expression" dxfId="516" priority="545">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="515" priority="546">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="514" priority="547">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="513" priority="548">
+    <cfRule type="expression" dxfId="518" priority="545">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="517" priority="546">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="516" priority="547">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="515" priority="548">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="512" priority="541">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="511" priority="542">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="510" priority="543">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="509" priority="544">
+    <cfRule type="expression" dxfId="514" priority="541">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="513" priority="542">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="512" priority="543">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="511" priority="544">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="508" priority="537">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="507" priority="538">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="506" priority="539">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="505" priority="540">
+    <cfRule type="expression" dxfId="510" priority="537">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="509" priority="538">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="508" priority="539">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="507" priority="540">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="504" priority="533">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="503" priority="534">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="502" priority="535">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="501" priority="536">
+    <cfRule type="expression" dxfId="506" priority="533">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="505" priority="534">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="504" priority="535">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="503" priority="536">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="expression" dxfId="500" priority="529">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="499" priority="530">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="498" priority="531">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="497" priority="532">
+    <cfRule type="expression" dxfId="502" priority="529">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="501" priority="530">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="500" priority="531">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="499" priority="532">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="496" priority="525">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="495" priority="526">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="494" priority="527">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="493" priority="528">
+    <cfRule type="expression" dxfId="498" priority="525">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="497" priority="526">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="496" priority="527">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="495" priority="528">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="expression" dxfId="492" priority="521">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="491" priority="522">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="490" priority="523">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="489" priority="524">
+    <cfRule type="expression" dxfId="494" priority="521">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="493" priority="522">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="492" priority="523">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="491" priority="524">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="488" priority="517">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="487" priority="518">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="486" priority="519">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="485" priority="520">
+    <cfRule type="expression" dxfId="490" priority="517">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="489" priority="518">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="488" priority="519">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="487" priority="520">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="484" priority="513">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="483" priority="514">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="482" priority="515">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="481" priority="516">
+    <cfRule type="expression" dxfId="486" priority="513">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="485" priority="514">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="484" priority="515">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="483" priority="516">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41">
-    <cfRule type="expression" dxfId="480" priority="509">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="479" priority="510">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="478" priority="511">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="477" priority="512">
+    <cfRule type="expression" dxfId="482" priority="509">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="481" priority="510">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="480" priority="511">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="479" priority="512">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="476" priority="505">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="475" priority="506">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="474" priority="507">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="473" priority="508">
+    <cfRule type="expression" dxfId="478" priority="505">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="477" priority="506">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="476" priority="507">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="475" priority="508">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="expression" dxfId="472" priority="501">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="471" priority="502">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="470" priority="503">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="469" priority="504">
+    <cfRule type="expression" dxfId="474" priority="501">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="473" priority="502">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="472" priority="503">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="471" priority="504">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="expression" dxfId="468" priority="497">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="467" priority="498">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="466" priority="499">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="465" priority="500">
+    <cfRule type="expression" dxfId="470" priority="497">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="469" priority="498">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="468" priority="499">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="467" priority="500">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="464" priority="493">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="463" priority="494">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="462" priority="495">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="461" priority="496">
+    <cfRule type="expression" dxfId="466" priority="493">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="465" priority="494">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="464" priority="495">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="463" priority="496">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="460" priority="489">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="459" priority="490">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="458" priority="491">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="457" priority="492">
+    <cfRule type="expression" dxfId="462" priority="489">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="461" priority="490">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="460" priority="491">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="459" priority="492">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="expression" dxfId="456" priority="485">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="455" priority="486">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="454" priority="487">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="453" priority="488">
+    <cfRule type="expression" dxfId="458" priority="485">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="457" priority="486">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="456" priority="487">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="455" priority="488">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="expression" dxfId="452" priority="481">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="451" priority="482">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="450" priority="483">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="449" priority="484">
+    <cfRule type="expression" dxfId="454" priority="481">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="453" priority="482">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="452" priority="483">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="451" priority="484">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="expression" dxfId="448" priority="477">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="447" priority="478">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="446" priority="479">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="445" priority="480">
+    <cfRule type="expression" dxfId="450" priority="477">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="449" priority="478">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="448" priority="479">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="447" priority="480">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45">
-    <cfRule type="expression" dxfId="444" priority="473">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="443" priority="474">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="442" priority="475">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="441" priority="476">
+    <cfRule type="expression" dxfId="446" priority="473">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="445" priority="474">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="444" priority="475">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="443" priority="476">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="expression" dxfId="440" priority="469">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="439" priority="470">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="438" priority="471">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="437" priority="472">
+    <cfRule type="expression" dxfId="442" priority="469">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="441" priority="470">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="440" priority="471">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="439" priority="472">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="expression" dxfId="436" priority="465">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="435" priority="466">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="434" priority="467">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="433" priority="468">
+    <cfRule type="expression" dxfId="438" priority="465">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="437" priority="466">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="436" priority="467">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="435" priority="468">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="expression" dxfId="432" priority="461">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="431" priority="462">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="430" priority="463">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="429" priority="464">
+    <cfRule type="expression" dxfId="434" priority="461">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="433" priority="462">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="432" priority="463">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="431" priority="464">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="expression" dxfId="428" priority="457">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="427" priority="458">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="426" priority="459">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="425" priority="460">
+    <cfRule type="expression" dxfId="430" priority="457">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="429" priority="458">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="428" priority="459">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="427" priority="460">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="424" priority="453">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="423" priority="454">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="422" priority="455">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="421" priority="456">
+    <cfRule type="expression" dxfId="426" priority="453">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="425" priority="454">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="424" priority="455">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="423" priority="456">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="420" priority="449">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="419" priority="450">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="418" priority="451">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="417" priority="452">
+    <cfRule type="expression" dxfId="422" priority="449">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="421" priority="450">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="420" priority="451">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="419" priority="452">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="416" priority="445">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="415" priority="446">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="414" priority="447">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="413" priority="448">
+    <cfRule type="expression" dxfId="418" priority="445">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="417" priority="446">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="416" priority="447">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="415" priority="448">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49">
-    <cfRule type="expression" dxfId="412" priority="441">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="411" priority="442">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="410" priority="443">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="409" priority="444">
+    <cfRule type="expression" dxfId="414" priority="441">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="413" priority="442">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="412" priority="443">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="411" priority="444">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="expression" dxfId="408" priority="437">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="407" priority="438">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="406" priority="439">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="405" priority="440">
+    <cfRule type="expression" dxfId="410" priority="437">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="409" priority="438">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="408" priority="439">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="407" priority="440">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="expression" dxfId="404" priority="433">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="403" priority="434">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="402" priority="435">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="401" priority="436">
+    <cfRule type="expression" dxfId="406" priority="433">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="405" priority="434">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="404" priority="435">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="403" priority="436">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="expression" dxfId="400" priority="429">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="399" priority="430">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="398" priority="431">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="397" priority="432">
+    <cfRule type="expression" dxfId="402" priority="429">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="401" priority="430">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="400" priority="431">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="399" priority="432">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="396" priority="425">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="395" priority="426">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="394" priority="427">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="393" priority="428">
+    <cfRule type="expression" dxfId="398" priority="425">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="397" priority="426">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="396" priority="427">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="395" priority="428">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="392" priority="421">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="391" priority="422">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="390" priority="423">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="389" priority="424">
+    <cfRule type="expression" dxfId="394" priority="421">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="393" priority="422">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="392" priority="423">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="391" priority="424">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="388" priority="417">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="387" priority="418">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="386" priority="419">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="385" priority="420">
+    <cfRule type="expression" dxfId="390" priority="417">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="389" priority="418">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="388" priority="419">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="387" priority="420">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="expression" dxfId="384" priority="413">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="383" priority="414">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="382" priority="415">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="381" priority="416">
+    <cfRule type="expression" dxfId="386" priority="413">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="385" priority="414">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="384" priority="415">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="383" priority="416">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52">
-    <cfRule type="expression" dxfId="380" priority="409">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="379" priority="410">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="378" priority="411">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="377" priority="412">
+    <cfRule type="expression" dxfId="382" priority="409">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="381" priority="410">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="380" priority="411">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="379" priority="412">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="376" priority="405">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="375" priority="406">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="374" priority="407">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="373" priority="408">
+    <cfRule type="expression" dxfId="378" priority="405">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="377" priority="406">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="376" priority="407">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="375" priority="408">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="expression" dxfId="372" priority="401">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="371" priority="402">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="370" priority="403">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="369" priority="404">
+    <cfRule type="expression" dxfId="374" priority="401">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="373" priority="402">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="372" priority="403">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="371" priority="404">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="expression" dxfId="368" priority="397">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="367" priority="398">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="366" priority="399">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="365" priority="400">
+    <cfRule type="expression" dxfId="370" priority="397">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="369" priority="398">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="368" priority="399">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="367" priority="400">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="expression" dxfId="364" priority="393">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="363" priority="394">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="362" priority="395">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="361" priority="396">
+    <cfRule type="expression" dxfId="366" priority="393">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="365" priority="394">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="364" priority="395">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="363" priority="396">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="expression" dxfId="360" priority="389">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="359" priority="390">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="358" priority="391">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="357" priority="392">
+    <cfRule type="expression" dxfId="362" priority="389">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="361" priority="390">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="360" priority="391">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="359" priority="392">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="expression" dxfId="356" priority="385">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="355" priority="386">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="354" priority="387">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="353" priority="388">
+    <cfRule type="expression" dxfId="358" priority="385">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="357" priority="386">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="356" priority="387">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="355" priority="388">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53">
-    <cfRule type="expression" dxfId="352" priority="381">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="351" priority="382">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="350" priority="383">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="349" priority="384">
+    <cfRule type="expression" dxfId="354" priority="381">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="353" priority="382">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="352" priority="383">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="351" priority="384">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="348" priority="377">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="347" priority="378">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="346" priority="379">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="345" priority="380">
+    <cfRule type="expression" dxfId="350" priority="377">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="349" priority="378">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="348" priority="379">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="347" priority="380">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="344" priority="373">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="343" priority="374">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="342" priority="375">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="341" priority="376">
+    <cfRule type="expression" dxfId="346" priority="373">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="345" priority="374">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="344" priority="375">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="343" priority="376">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33 C13:D13 D6:D8 C12 D14:D16 D37:D40 C41 C43 D44 C47:D47 C42:D42 D24">
-    <cfRule type="expression" dxfId="340" priority="361">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="339" priority="362">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="338" priority="363">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="337" priority="364">
+    <cfRule type="expression" dxfId="342" priority="361">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="341" priority="362">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="340" priority="363">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="339" priority="364">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:D10 C17:D17 C19:D19 D20 C21:D21 C36:D36 C9 C35 C2:D4">
-    <cfRule type="expression" dxfId="336" priority="369">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="335" priority="370">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="334" priority="371">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="333" priority="372">
+    <cfRule type="expression" dxfId="338" priority="369">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="337" priority="370">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="336" priority="371">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="335" priority="372">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="332" priority="357">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="331" priority="358">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="330" priority="359">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="329" priority="360">
+    <cfRule type="expression" dxfId="334" priority="357">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="333" priority="358">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="332" priority="359">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="331" priority="360">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="328" priority="353">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="327" priority="354">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="326" priority="355">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="325" priority="356">
+    <cfRule type="expression" dxfId="330" priority="353">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="329" priority="354">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="328" priority="355">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="327" priority="356">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="324" priority="349">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="323" priority="350">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="322" priority="351">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="321" priority="352">
+    <cfRule type="expression" dxfId="326" priority="349">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="325" priority="350">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="324" priority="351">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="323" priority="352">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="320" priority="345">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="319" priority="346">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="318" priority="347">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="317" priority="348">
+    <cfRule type="expression" dxfId="322" priority="345">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="321" priority="346">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="320" priority="347">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="319" priority="348">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="316" priority="341">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="315" priority="342">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="314" priority="343">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="313" priority="344">
+    <cfRule type="expression" dxfId="318" priority="341">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="317" priority="342">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="316" priority="343">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="315" priority="344">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="312" priority="337">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="311" priority="338">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="310" priority="339">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="309" priority="340">
+    <cfRule type="expression" dxfId="314" priority="337">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="313" priority="338">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="312" priority="339">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="311" priority="340">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="308" priority="333">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="307" priority="334">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="306" priority="335">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="305" priority="336">
+    <cfRule type="expression" dxfId="310" priority="333">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="309" priority="334">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="308" priority="335">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="307" priority="336">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="304" priority="329">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="303" priority="330">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="302" priority="331">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="301" priority="332">
+    <cfRule type="expression" dxfId="306" priority="329">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="305" priority="330">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="304" priority="331">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="303" priority="332">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="300" priority="321">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="299" priority="322">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="298" priority="323">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="297" priority="324">
+    <cfRule type="expression" dxfId="302" priority="321">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="301" priority="322">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="300" priority="323">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="299" priority="324">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="296" priority="317">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="295" priority="318">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="294" priority="319">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="293" priority="320">
+    <cfRule type="expression" dxfId="298" priority="317">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="297" priority="318">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="296" priority="319">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="295" priority="320">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="292" priority="313">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="291" priority="314">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="290" priority="315">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="289" priority="316">
+    <cfRule type="expression" dxfId="294" priority="313">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="293" priority="314">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="292" priority="315">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="291" priority="316">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="288" priority="309">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="287" priority="310">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="286" priority="311">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="285" priority="312">
+    <cfRule type="expression" dxfId="290" priority="309">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="289" priority="310">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="288" priority="311">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="287" priority="312">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="284" priority="305">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="283" priority="306">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="282" priority="307">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="281" priority="308">
+    <cfRule type="expression" dxfId="286" priority="305">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="285" priority="306">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="284" priority="307">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="283" priority="308">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="280" priority="301">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="279" priority="302">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="278" priority="303">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="277" priority="304">
+    <cfRule type="expression" dxfId="282" priority="301">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="281" priority="302">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="280" priority="303">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="279" priority="304">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="276" priority="297">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="275" priority="298">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="274" priority="299">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="273" priority="300">
+    <cfRule type="expression" dxfId="278" priority="297">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="277" priority="298">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="276" priority="299">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="275" priority="300">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="272" priority="293">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="271" priority="294">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="270" priority="295">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="269" priority="296">
+    <cfRule type="expression" dxfId="274" priority="293">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="273" priority="294">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="272" priority="295">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="271" priority="296">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="268" priority="289">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="267" priority="290">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="266" priority="291">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="265" priority="292">
+    <cfRule type="expression" dxfId="270" priority="289">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="269" priority="290">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="268" priority="291">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="267" priority="292">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="264" priority="285">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="263" priority="286">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="262" priority="287">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="261" priority="288">
+    <cfRule type="expression" dxfId="266" priority="285">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="265" priority="286">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="264" priority="287">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="263" priority="288">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="260" priority="281">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="259" priority="282">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="258" priority="283">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="257" priority="284">
+    <cfRule type="expression" dxfId="262" priority="281">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="261" priority="282">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="260" priority="283">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="259" priority="284">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="256" priority="269">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="255" priority="270">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="254" priority="271">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="253" priority="272">
+    <cfRule type="expression" dxfId="258" priority="269">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="257" priority="270">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="256" priority="271">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="255" priority="272">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="252" priority="253">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="251" priority="254">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="250" priority="255">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="249" priority="256">
+    <cfRule type="expression" dxfId="254" priority="253">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="253" priority="254">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="252" priority="255">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="251" priority="256">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="248" priority="249">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="247" priority="250">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="246" priority="251">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="245" priority="252">
+    <cfRule type="expression" dxfId="250" priority="249">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="249" priority="250">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="248" priority="251">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="247" priority="252">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="244" priority="245">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="243" priority="246">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="242" priority="247">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="241" priority="248">
+    <cfRule type="expression" dxfId="246" priority="245">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="245" priority="246">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="244" priority="247">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="243" priority="248">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="240" priority="241">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="239" priority="242">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="238" priority="243">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="237" priority="244">
+    <cfRule type="expression" dxfId="242" priority="241">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="241" priority="242">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="240" priority="243">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="239" priority="244">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="236" priority="237">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="235" priority="238">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="234" priority="239">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="233" priority="240">
+    <cfRule type="expression" dxfId="238" priority="237">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="237" priority="238">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="236" priority="239">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="235" priority="240">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="232" priority="233">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="231" priority="234">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="230" priority="235">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="229" priority="236">
+    <cfRule type="expression" dxfId="234" priority="233">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="233" priority="234">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="232" priority="235">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="231" priority="236">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="228" priority="229">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="227" priority="230">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="226" priority="231">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="225" priority="232">
+    <cfRule type="expression" dxfId="230" priority="229">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="229" priority="230">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="228" priority="231">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="227" priority="232">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="224" priority="225">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="223" priority="226">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="222" priority="227">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="221" priority="228">
+    <cfRule type="expression" dxfId="226" priority="225">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="225" priority="226">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="224" priority="227">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="223" priority="228">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="220" priority="221">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="219" priority="222">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="218" priority="223">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="217" priority="224">
+    <cfRule type="expression" dxfId="222" priority="221">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="221" priority="222">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="220" priority="223">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="219" priority="224">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="216" priority="217">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="215" priority="218">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="214" priority="219">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="213" priority="220">
+    <cfRule type="expression" dxfId="218" priority="217">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="217" priority="218">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="216" priority="219">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="215" priority="220">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="212" priority="213">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="211" priority="214">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="210" priority="215">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="209" priority="216">
+    <cfRule type="expression" dxfId="214" priority="213">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="213" priority="214">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="212" priority="215">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="211" priority="216">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="208" priority="209">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="207" priority="210">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="206" priority="211">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="205" priority="212">
+    <cfRule type="expression" dxfId="210" priority="209">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="209" priority="210">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="208" priority="211">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="207" priority="212">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48">
-    <cfRule type="expression" dxfId="204" priority="205">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="203" priority="206">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="202" priority="207">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="201" priority="208">
+    <cfRule type="expression" dxfId="206" priority="205">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="205" priority="206">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="204" priority="207">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="203" priority="208">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="200" priority="201">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="199" priority="202">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="198" priority="203">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="197" priority="204">
+    <cfRule type="expression" dxfId="202" priority="201">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="201" priority="202">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="200" priority="203">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="199" priority="204">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="196" priority="197">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="195" priority="198">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="194" priority="199">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="193" priority="200">
+    <cfRule type="expression" dxfId="198" priority="197">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="197" priority="198">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="196" priority="199">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="195" priority="200">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="192" priority="193">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="191" priority="194">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="190" priority="195">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="189" priority="196">
+    <cfRule type="expression" dxfId="194" priority="193">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="193" priority="194">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="192" priority="195">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="191" priority="196">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="188" priority="189">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="187" priority="190">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="186" priority="191">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="185" priority="192">
+    <cfRule type="expression" dxfId="190" priority="189">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="189" priority="190">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="188" priority="191">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="187" priority="192">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="184" priority="185">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="183" priority="186">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="182" priority="187">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="181" priority="188">
+    <cfRule type="expression" dxfId="186" priority="185">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="185" priority="186">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="184" priority="187">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="183" priority="188">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="180" priority="181">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="179" priority="182">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="178" priority="183">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="177" priority="184">
+    <cfRule type="expression" dxfId="182" priority="181">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="181" priority="182">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="180" priority="183">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="179" priority="184">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="176" priority="177">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="175" priority="178">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="174" priority="179">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="173" priority="180">
+    <cfRule type="expression" dxfId="178" priority="177">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="177" priority="178">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="176" priority="179">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="175" priority="180">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="172" priority="173">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="171" priority="174">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="170" priority="175">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="169" priority="176">
+    <cfRule type="expression" dxfId="174" priority="173">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="173" priority="174">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="175">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="171" priority="176">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="168" priority="169">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="167" priority="170">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="166" priority="171">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="165" priority="172">
+    <cfRule type="expression" dxfId="170" priority="169">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="169" priority="170">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="168" priority="171">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="167" priority="172">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="164" priority="165">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="163" priority="166">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="162" priority="167">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="161" priority="168">
+    <cfRule type="expression" dxfId="166" priority="165">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="165" priority="166">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="164" priority="167">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="163" priority="168">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="160" priority="161">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="159" priority="162">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="158" priority="163">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="157" priority="164">
+    <cfRule type="expression" dxfId="162" priority="161">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="161" priority="162">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="163">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="159" priority="164">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="156" priority="149">
+    <cfRule type="expression" dxfId="158" priority="149">
       <formula>$L31="Available"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="150">
+    <cfRule type="expression" dxfId="157" priority="150">
       <formula>$L31="Open AR"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="151">
+    <cfRule type="expression" dxfId="156" priority="151">
       <formula>$L31="Quote requested"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="152">
+    <cfRule type="expression" dxfId="155" priority="152">
       <formula>$L31="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:E28">
-    <cfRule type="expression" dxfId="152" priority="141">
+    <cfRule type="expression" dxfId="154" priority="141">
       <formula>$L27="Available"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="142">
+    <cfRule type="expression" dxfId="153" priority="142">
       <formula>$L27="Open AR"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="143">
+    <cfRule type="expression" dxfId="152" priority="143">
       <formula>$L27="Quote requested"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="144">
+    <cfRule type="expression" dxfId="151" priority="144">
       <formula>$L27="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="148" priority="137">
+    <cfRule type="expression" dxfId="150" priority="137">
       <formula>$L29="Available"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="138">
+    <cfRule type="expression" dxfId="149" priority="138">
       <formula>$L29="Open AR"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="139">
+    <cfRule type="expression" dxfId="148" priority="139">
       <formula>$L29="Quote requested"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="140">
+    <cfRule type="expression" dxfId="147" priority="140">
       <formula>$L29="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="144" priority="133">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="143" priority="134">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="142" priority="135">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="141" priority="136">
+    <cfRule type="expression" dxfId="146" priority="133">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="134">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="135">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="136">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="140" priority="129">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="139" priority="130">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="138" priority="131">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="137" priority="132">
+    <cfRule type="expression" dxfId="142" priority="129">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="130">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="131">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="132">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="136" priority="125">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="126">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="127">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="133" priority="128">
+    <cfRule type="expression" dxfId="138" priority="125">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="137" priority="126">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="127">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="135" priority="128">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="132" priority="121">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="131" priority="122">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="123">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="129" priority="124">
+    <cfRule type="expression" dxfId="134" priority="121">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="122">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="123">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="124">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="128" priority="117">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="127" priority="118">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="119">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="120">
+    <cfRule type="expression" dxfId="130" priority="117">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="129" priority="118">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="119">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="127" priority="120">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="124" priority="113">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="123" priority="114">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="122" priority="115">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="121" priority="116">
+    <cfRule type="expression" dxfId="126" priority="113">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="114">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="115">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="116">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="120" priority="109">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="110">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="111">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="112">
+    <cfRule type="expression" dxfId="122" priority="109">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="110">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="111">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="119" priority="112">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="116" priority="105">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="106">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="107">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="113" priority="108">
+    <cfRule type="expression" dxfId="118" priority="105">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="106">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="107">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="108">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="112" priority="101">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="102">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="103">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="104">
+    <cfRule type="expression" dxfId="114" priority="101">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="102">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="103">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="104">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="108" priority="97">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="98">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="99">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="100">
+    <cfRule type="expression" dxfId="110" priority="97">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="98">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="99">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="100">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="104" priority="89">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="90">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="91">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="92">
+    <cfRule type="expression" dxfId="106" priority="89">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="90">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="91">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="92">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="100" priority="85">
+    <cfRule type="expression" dxfId="102" priority="85">
       <formula>$L26="Available"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="86">
+    <cfRule type="expression" dxfId="101" priority="86">
       <formula>$L26="Open AR"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="87">
+    <cfRule type="expression" dxfId="100" priority="87">
       <formula>$L26="Quote requested"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="88">
+    <cfRule type="expression" dxfId="99" priority="88">
       <formula>$L26="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="96" priority="81">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="95" priority="82">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="83">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="93" priority="84">
+    <cfRule type="expression" dxfId="98" priority="81">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="82">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="83">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="84">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="92" priority="77">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="78">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="79">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="80">
+    <cfRule type="expression" dxfId="94" priority="77">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="78">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="79">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="80">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="88" priority="73">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="87" priority="74">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="75">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="76">
+    <cfRule type="expression" dxfId="90" priority="73">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="74">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="75">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="76">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="84" priority="69">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="70">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="71">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="72">
+    <cfRule type="expression" dxfId="86" priority="69">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="70">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="71">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="72">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="80" priority="61">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="62">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="63">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="64">
+    <cfRule type="expression" dxfId="82" priority="61">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="62">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="63">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="64">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="76" priority="57">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="58">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="59">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="60">
+    <cfRule type="expression" dxfId="78" priority="57">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="58">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="59">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="60">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="72" priority="53">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="54">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="55">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="56">
+    <cfRule type="expression" dxfId="74" priority="53">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="54">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="55">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="56">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="68" priority="49">
+    <cfRule type="expression" dxfId="70" priority="49">
       <formula>$L32="Available"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="50">
+    <cfRule type="expression" dxfId="69" priority="50">
       <formula>$L32="Open AR"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="51">
+    <cfRule type="expression" dxfId="68" priority="51">
       <formula>$L32="Quote requested"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="52">
+    <cfRule type="expression" dxfId="67" priority="52">
       <formula>$L32="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="64" priority="45">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="46">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="47">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="48">
+    <cfRule type="expression" dxfId="66" priority="45">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="46">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="47">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="48">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="60" priority="41">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="42">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="43">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="44">
+    <cfRule type="expression" dxfId="62" priority="41">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="42">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="43">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="44">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="56" priority="37">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="38">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="39">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="40">
+    <cfRule type="expression" dxfId="58" priority="37">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="38">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="39">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="40">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="52" priority="33">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="34">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="35">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="36">
+    <cfRule type="expression" dxfId="54" priority="33">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="34">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="35">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="36">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="48" priority="29">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="30">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="31">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="32">
+    <cfRule type="expression" dxfId="50" priority="29">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="30">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="31">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="32">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="44" priority="25">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="26">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="27">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="28">
+    <cfRule type="expression" dxfId="46" priority="25">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="26">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="27">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="28">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="40" priority="21">
+    <cfRule type="expression" dxfId="42" priority="21">
       <formula>$L28="Available"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="22">
+    <cfRule type="expression" dxfId="41" priority="22">
       <formula>$L28="Open AR"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="23">
+    <cfRule type="expression" dxfId="40" priority="23">
       <formula>$L28="Quote requested"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="24">
+    <cfRule type="expression" dxfId="39" priority="24">
       <formula>$L28="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="36" priority="17">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="18">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="19">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="20">
+    <cfRule type="expression" dxfId="38" priority="17">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="18">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="19">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="20">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="32" priority="13">
+    <cfRule type="expression" dxfId="34" priority="13">
       <formula>$L30="Available"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="14">
+    <cfRule type="expression" dxfId="33" priority="14">
       <formula>$L30="Open AR"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="15">
+    <cfRule type="expression" dxfId="32" priority="15">
       <formula>$L30="Quote requested"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="16">
+    <cfRule type="expression" dxfId="31" priority="16">
       <formula>$L30="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="28" priority="9">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="10">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="11">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="12">
+    <cfRule type="expression" dxfId="30" priority="9">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="10">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="11">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="12">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="24" priority="5">
-      <formula>#REF!="Available"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="6">
-      <formula>#REF!="Open AR"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="7">
-      <formula>#REF!="Quote requested"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="8">
+    <cfRule type="expression" dxfId="26" priority="5">
+      <formula>#REF!="Available"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="6">
+      <formula>#REF!="Open AR"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="7">
+      <formula>#REF!="Quote requested"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="8">
       <formula>#REF!="Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9852,7 +10135,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7E36950-EEC1-4CFD-B9DB-54F5583C925E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4457EAE-32E5-4B8A-BCA4-51B2A2AD572B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="HelblingDocs"/>

</xml_diff>